<commit_message>
Config, constants and log directory added, changes happen to different files for the code reduction purpose
</commit_message>
<xml_diff>
--- a/TestData/Register_page.xlsx
+++ b/TestData/Register_page.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mohni\PycharmProjects\cchc_automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CE966E6-1D23-41FE-9332-1FB9FBFDD934}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{032D7679-EDAD-44C2-B1A6-1F5C580A1AD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>name</t>
   </si>
@@ -39,69 +39,15 @@
     <t>address</t>
   </si>
   <si>
-    <t>adhar_no</t>
-  </si>
-  <si>
     <t>password</t>
   </si>
   <si>
     <t>Cpassword</t>
   </si>
   <si>
-    <t>file_path</t>
-  </si>
-  <si>
-    <t>pass1</t>
-  </si>
-  <si>
-    <t>pass2</t>
-  </si>
-  <si>
-    <t>short_pass</t>
-  </si>
-  <si>
-    <t>C:\Users\mohni\Downloads\Sign mohni updated.jpg</t>
-  </si>
-  <si>
-    <t>Weak_pass</t>
-  </si>
-  <si>
-    <t>Weak_Cpass</t>
-  </si>
-  <si>
-    <t>New_email</t>
-  </si>
-  <si>
-    <t>New_phone</t>
-  </si>
-  <si>
     <t>Sagar</t>
   </si>
   <si>
-    <t>Inv_email</t>
-  </si>
-  <si>
-    <t>New_email1</t>
-  </si>
-  <si>
-    <t>New_phone1</t>
-  </si>
-  <si>
-    <t>New_email2</t>
-  </si>
-  <si>
-    <t>New_phone2</t>
-  </si>
-  <si>
-    <t>New_email3</t>
-  </si>
-  <si>
-    <t>New_phone3</t>
-  </si>
-  <si>
-    <t>short_Cpass</t>
-  </si>
-  <si>
     <t>Tanu</t>
   </si>
   <si>
@@ -109,33 +55,12 @@
   </si>
   <si>
     <t>Tanu@1234</t>
-  </si>
-  <si>
-    <t>tanu123@gmail.com</t>
-  </si>
-  <si>
-    <t>tanu456@gmail.com</t>
-  </si>
-  <si>
-    <t>Tanu@12345</t>
-  </si>
-  <si>
-    <t>tanu789@gmail.com</t>
-  </si>
-  <si>
-    <t>tanu714@gmail.com</t>
-  </si>
-  <si>
-    <t>tanu</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="00000"/>
-  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -182,10 +107,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -468,10 +392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="V2" sqref="V2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -480,180 +404,56 @@
     <col min="2" max="2" width="16.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="44.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="N1" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="W1" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="C2">
         <v>6260458978</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="2">
-        <v>326598741485</v>
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J2">
-        <v>12345</v>
-      </c>
-      <c r="K2">
-        <v>6260852963</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="M2" s="1">
-        <v>6260123985</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q2">
-        <v>6260854796</v>
-      </c>
-      <c r="R2" t="s">
-        <v>33</v>
-      </c>
-      <c r="S2" t="s">
-        <v>33</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="U2">
-        <v>6260854967</v>
-      </c>
-      <c r="V2">
-        <v>12345</v>
-      </c>
-      <c r="W2">
-        <v>12345</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{3F1F1C84-7E5D-4AAF-951A-8B1F1D9AAC64}"/>
-    <hyperlink ref="F2" r:id="rId2" xr:uid="{6EEB4880-88BE-461A-B800-60472A6D0B55}"/>
-    <hyperlink ref="G2" r:id="rId3" xr:uid="{7269FE13-7639-4839-841C-9BFEDB232A3A}"/>
-    <hyperlink ref="I2" r:id="rId4" xr:uid="{B0F6D314-5070-4BC9-A17D-59A782A196F5}"/>
-    <hyperlink ref="L2" r:id="rId5" xr:uid="{B9B431D4-3B8C-4F05-8625-5210478399BB}"/>
-    <hyperlink ref="N2" r:id="rId6" xr:uid="{E12F03DE-73FC-4042-B744-5BD085E2060E}"/>
-    <hyperlink ref="O2" r:id="rId7" xr:uid="{2F67B2A2-4881-4863-8300-C7294C6A8447}"/>
-    <hyperlink ref="P2" r:id="rId8" xr:uid="{5DEEAA15-CDF0-4EAD-97F2-09AFDAD85F25}"/>
-    <hyperlink ref="T2" r:id="rId9" xr:uid="{AF65C321-BFAC-4840-9FBA-EAE20D028141}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{6EEB4880-88BE-461A-B800-60472A6D0B55}"/>
+    <hyperlink ref="F2" r:id="rId3" xr:uid="{7269FE13-7639-4839-841C-9BFEDB232A3A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId10"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>